<commit_message>
Add CI workflow, .gitignore, and documentation files; enhance report generation and testing
</commit_message>
<xml_diff>
--- a/assets/employees.xlsx
+++ b/assets/employees.xlsx
@@ -1,31 +1,370 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc4b80da33a699eb/Documents/my codess/Reads-the-Excel-file-and-returns-it-as-a-pandas-DataFrame/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc4b80da33a699eb/Documents/my codess/employee-report-generator/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_55C36EED8B5C5051A9DB2B953999E256863B40F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0543AF9F-21E5-4ECB-BAD9-3BB6BE79795A}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{0ED0E228-CE21-4D4C-84BC-A0C29101BA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05F2740F-5467-4FDA-8F8D-45EB2B6C8DA1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Employee Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Item Purchases" sheetId="2" r:id="rId2"/>
+    <sheet name="Employee Data" sheetId="2" r:id="rId1"/>
+    <sheet name="Item Purchases" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="144">
   <si>
     <t>Employee Name</t>
   </si>
   <si>
+    <t>Item Purchased</t>
+  </si>
+  <si>
+    <t>Purchase Date</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price (INR)</t>
+  </si>
+  <si>
+    <t>Total Cost (INR)</t>
+  </si>
+  <si>
+    <t>Avinesh Masih</t>
+  </si>
+  <si>
+    <t>Anshika Singh</t>
+  </si>
+  <si>
+    <t>Rohan Kapoor</t>
+  </si>
+  <si>
+    <t>Anika Reddy</t>
+  </si>
+  <si>
+    <t>Dev Patel</t>
+  </si>
+  <si>
+    <t>Kavya Iyer</t>
+  </si>
+  <si>
+    <t>Aarav Singhania</t>
+  </si>
+  <si>
+    <t>Zara Nair</t>
+  </si>
+  <si>
+    <t>Krishna Menon</t>
+  </si>
+  <si>
+    <t>Anaya Deshmukh</t>
+  </si>
+  <si>
+    <t>Vihaan Chatterjee</t>
+  </si>
+  <si>
+    <t>Ishani Gupta</t>
+  </si>
+  <si>
+    <t>Aditya Verma</t>
+  </si>
+  <si>
+    <t>Maya Krishnamurthy</t>
+  </si>
+  <si>
+    <t>Kabir Mehra</t>
+  </si>
+  <si>
+    <t>Riya Srinivasan</t>
+  </si>
+  <si>
+    <t>Virat Bose</t>
+  </si>
+  <si>
+    <t>Nisha Ranganathan</t>
+  </si>
+  <si>
+    <t>Shiv Joshi</t>
+  </si>
+  <si>
+    <t>Meera Ahuja</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Smartphone</t>
+  </si>
+  <si>
+    <t>Headphones</t>
+  </si>
+  <si>
+    <t>Keyboard</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>Tablet</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>Printer</t>
+  </si>
+  <si>
+    <t>Speakers</t>
+  </si>
+  <si>
+    <t>Smartwatch</t>
+  </si>
+  <si>
+    <t>External HDD</t>
+  </si>
+  <si>
+    <t>Desk Chair</t>
+  </si>
+  <si>
+    <t>USB Drive</t>
+  </si>
+  <si>
+    <t>Webcam</t>
+  </si>
+  <si>
+    <t>2025-01-05</t>
+  </si>
+  <si>
+    <t>2025-01-10</t>
+  </si>
+  <si>
+    <t>2025-01-15</t>
+  </si>
+  <si>
+    <t>2025-01-20</t>
+  </si>
+  <si>
+    <t>2025-01-25</t>
+  </si>
+  <si>
+    <t>2025-01-30</t>
+  </si>
+  <si>
+    <t>2025-02-05</t>
+  </si>
+  <si>
+    <t>2025-02-10</t>
+  </si>
+  <si>
+    <t>2025-02-15</t>
+  </si>
+  <si>
+    <t>2025-02-20</t>
+  </si>
+  <si>
+    <t>2025-02-25</t>
+  </si>
+  <si>
+    <t>2025-03-01</t>
+  </si>
+  <si>
+    <t>2025-03-05</t>
+  </si>
+  <si>
+    <t>2025-03-10</t>
+  </si>
+  <si>
+    <t>2025-03-15</t>
+  </si>
+  <si>
+    <t>2025-03-20</t>
+  </si>
+  <si>
+    <t>2025-03-25</t>
+  </si>
+  <si>
+    <t>2025-03-30</t>
+  </si>
+  <si>
+    <t>2025-04-05</t>
+  </si>
+  <si>
+    <t>2025-04-10</t>
+  </si>
+  <si>
+    <t>2025-01-16</t>
+  </si>
+  <si>
+    <t>2025-01-31</t>
+  </si>
+  <si>
+    <t>2025-01-26</t>
+  </si>
+  <si>
+    <t>2025-01-09</t>
+  </si>
+  <si>
+    <t>2025-02-09</t>
+  </si>
+  <si>
+    <t>2025-01-13</t>
+  </si>
+  <si>
+    <t>2025-01-11</t>
+  </si>
+  <si>
+    <t>2025-01-17</t>
+  </si>
+  <si>
+    <t>2025-02-01</t>
+  </si>
+  <si>
+    <t>2025-02-12</t>
+  </si>
+  <si>
+    <t>2025-01-29</t>
+  </si>
+  <si>
+    <t>2025-01-28</t>
+  </si>
+  <si>
+    <t>2025-02-21</t>
+  </si>
+  <si>
+    <t>2025-02-24</t>
+  </si>
+  <si>
+    <t>2025-02-08</t>
+  </si>
+  <si>
+    <t>2025-03-03</t>
+  </si>
+  <si>
+    <t>2025-02-11</t>
+  </si>
+  <si>
+    <t>2025-03-02</t>
+  </si>
+  <si>
+    <t>2025-02-16</t>
+  </si>
+  <si>
+    <t>2025-03-07</t>
+  </si>
+  <si>
+    <t>2025-02-28</t>
+  </si>
+  <si>
+    <t>2025-03-17</t>
+  </si>
+  <si>
+    <t>2025-03-04</t>
+  </si>
+  <si>
+    <t>2025-03-13</t>
+  </si>
+  <si>
+    <t>2025-03-11</t>
+  </si>
+  <si>
+    <t>2025-03-06</t>
+  </si>
+  <si>
+    <t>2025-03-08</t>
+  </si>
+  <si>
+    <t>2025-03-27</t>
+  </si>
+  <si>
+    <t>2025-03-16</t>
+  </si>
+  <si>
+    <t>2025-03-14</t>
+  </si>
+  <si>
+    <t>2025-03-26</t>
+  </si>
+  <si>
+    <t>2025-03-23</t>
+  </si>
+  <si>
+    <t>2025-03-28</t>
+  </si>
+  <si>
+    <t>2025-04-03</t>
+  </si>
+  <si>
+    <t>2025-03-29</t>
+  </si>
+  <si>
+    <t>2025-03-21</t>
+  </si>
+  <si>
+    <t>2025-03-24</t>
+  </si>
+  <si>
+    <t>2025-04-14</t>
+  </si>
+  <si>
+    <t>2025-04-06</t>
+  </si>
+  <si>
+    <t>2025-04-13</t>
+  </si>
+  <si>
+    <t>2025-04-17</t>
+  </si>
+  <si>
+    <t>2025-04-18</t>
+  </si>
+  <si>
+    <t>2025-04-09</t>
+  </si>
+  <si>
+    <t>2025-04-07</t>
+  </si>
+  <si>
+    <t>2025-04-15</t>
+  </si>
+  <si>
+    <t>2025-04-23</t>
+  </si>
+  <si>
+    <t>2025-04-27</t>
+  </si>
+  <si>
+    <t>2025-04-19</t>
+  </si>
+  <si>
+    <t>2025-04-12</t>
+  </si>
+  <si>
+    <t>2025-05-03</t>
+  </si>
+  <si>
+    <t>2025-04-26</t>
+  </si>
+  <si>
+    <t>2025-04-29</t>
+  </si>
+  <si>
+    <t>2025-04-24</t>
+  </si>
+  <si>
     <t>Age</t>
   </si>
   <si>
@@ -38,247 +377,82 @@
     <t>Salary (INR)</t>
   </si>
   <si>
-    <t>Avinesh Masih</t>
-  </si>
-  <si>
     <t>IT</t>
   </si>
   <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
     <t>Data Analyst</t>
   </si>
   <si>
-    <t>Anshika Singh</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
     <t>HR Manager</t>
   </si>
   <si>
-    <t>Rohan Kapoor</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
     <t>Marketing Head</t>
   </si>
   <si>
-    <t>Anika Reddy</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
     <t>Sales Manager</t>
   </si>
   <si>
-    <t>Dev Patel</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
     <t>Finance Director</t>
   </si>
   <si>
-    <t>Kavya Iyer</t>
-  </si>
-  <si>
-    <t>Operations</t>
-  </si>
-  <si>
     <t>Operations Manager</t>
   </si>
   <si>
-    <t>Aarav Singhania</t>
-  </si>
-  <si>
     <t>Data Scientist</t>
   </si>
   <si>
-    <t>Zara Nair</t>
-  </si>
-  <si>
     <t>HR Specialist</t>
   </si>
   <si>
-    <t>Krishna Menon</t>
-  </si>
-  <si>
     <t>Sales Executive</t>
   </si>
   <si>
-    <t>Anaya Deshmukh</t>
-  </si>
-  <si>
     <t>Marketing Analyst</t>
   </si>
   <si>
-    <t>Vihaan Chatterjee</t>
-  </si>
-  <si>
     <t>Financial Analyst</t>
   </si>
   <si>
-    <t>Ishani Gupta</t>
-  </si>
-  <si>
     <t>Operations Coordinator</t>
   </si>
   <si>
-    <t>Aditya Verma</t>
-  </si>
-  <si>
     <t>System Administrator</t>
   </si>
   <si>
-    <t>Maya Krishnamurthy</t>
-  </si>
-  <si>
     <t>Recruiter</t>
   </si>
   <si>
-    <t>Kabir Mehra</t>
-  </si>
-  <si>
     <t>Sales Associate</t>
   </si>
   <si>
-    <t>Riya Srinivasan</t>
-  </si>
-  <si>
     <t>Brand Manager</t>
   </si>
   <si>
-    <t>Virat Bose</t>
-  </si>
-  <si>
     <t>Financial Planner</t>
   </si>
   <si>
-    <t>Nisha Ranganathan</t>
-  </si>
-  <si>
     <t>Logistics Manager</t>
   </si>
   <si>
-    <t>Shiv Joshi</t>
-  </si>
-  <si>
     <t>IT Support</t>
   </si>
   <si>
-    <t>Meera Ahuja</t>
-  </si>
-  <si>
     <t>HR Coordinator</t>
-  </si>
-  <si>
-    <t>Item Purchased</t>
-  </si>
-  <si>
-    <t>Purchase Date</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Price (INR)</t>
-  </si>
-  <si>
-    <t>Total Cost (INR)</t>
-  </si>
-  <si>
-    <t>Laptop</t>
-  </si>
-  <si>
-    <t>2025-01-05</t>
-  </si>
-  <si>
-    <t>Smartphone</t>
-  </si>
-  <si>
-    <t>2025-01-10</t>
-  </si>
-  <si>
-    <t>Headphones</t>
-  </si>
-  <si>
-    <t>2025-01-15</t>
-  </si>
-  <si>
-    <t>Keyboard</t>
-  </si>
-  <si>
-    <t>2025-01-20</t>
-  </si>
-  <si>
-    <t>Mouse</t>
-  </si>
-  <si>
-    <t>2025-01-25</t>
-  </si>
-  <si>
-    <t>Monitor</t>
-  </si>
-  <si>
-    <t>2025-01-30</t>
-  </si>
-  <si>
-    <t>Tablet</t>
-  </si>
-  <si>
-    <t>2025-02-05</t>
-  </si>
-  <si>
-    <t>Camera</t>
-  </si>
-  <si>
-    <t>2025-02-10</t>
-  </si>
-  <si>
-    <t>Printer</t>
-  </si>
-  <si>
-    <t>2025-02-15</t>
-  </si>
-  <si>
-    <t>Speakers</t>
-  </si>
-  <si>
-    <t>2025-02-20</t>
-  </si>
-  <si>
-    <t>2025-02-25</t>
-  </si>
-  <si>
-    <t>2025-03-01</t>
-  </si>
-  <si>
-    <t>2025-03-05</t>
-  </si>
-  <si>
-    <t>2025-03-10</t>
-  </si>
-  <si>
-    <t>2025-03-15</t>
-  </si>
-  <si>
-    <t>2025-03-20</t>
-  </si>
-  <si>
-    <t>2025-03-25</t>
-  </si>
-  <si>
-    <t>2025-03-30</t>
-  </si>
-  <si>
-    <t>2025-04-05</t>
-  </si>
-  <si>
-    <t>2025-04-10</t>
   </si>
 </sst>
 </file>
@@ -296,7 +470,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -357,9 +534,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -397,7 +574,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -431,6 +608,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -465,9 +643,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -640,50 +819,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>114</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>124</v>
       </c>
       <c r="E2">
         <v>50000</v>
@@ -691,16 +862,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>125</v>
       </c>
       <c r="E3">
         <v>45000</v>
@@ -708,16 +879,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="E4">
         <v>70000</v>
@@ -725,16 +896,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>127</v>
       </c>
       <c r="E5">
         <v>60000</v>
@@ -742,16 +913,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>128</v>
       </c>
       <c r="E6">
         <v>75000</v>
@@ -759,16 +930,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="E7">
         <v>40000</v>
@@ -776,16 +947,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>130</v>
       </c>
       <c r="E8">
         <v>55000</v>
@@ -793,16 +964,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="E9">
         <v>43000</v>
@@ -810,16 +981,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>132</v>
       </c>
       <c r="E10">
         <v>62000</v>
@@ -827,16 +998,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
       <c r="E11">
         <v>70000</v>
@@ -844,16 +1015,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>134</v>
       </c>
       <c r="E12">
         <v>72000</v>
@@ -861,16 +1032,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="E13">
         <v>48000</v>
@@ -878,16 +1049,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>136</v>
       </c>
       <c r="E14">
         <v>50000</v>
@@ -895,16 +1066,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>137</v>
       </c>
       <c r="E15">
         <v>45000</v>
@@ -912,16 +1083,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>138</v>
       </c>
       <c r="E16">
         <v>60000</v>
@@ -929,16 +1100,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="E17">
         <v>65000</v>
@@ -946,16 +1117,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>140</v>
       </c>
       <c r="E18">
         <v>69000</v>
@@ -963,16 +1134,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>141</v>
       </c>
       <c r="E19">
         <v>70000</v>
@@ -980,16 +1151,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B20">
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>142</v>
       </c>
       <c r="E20">
         <v>55000</v>
@@ -997,42 +1168,36 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B21">
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="E21">
         <v>50000</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.5546875" customWidth="1"/>
-    <col min="2" max="2" width="32.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
-    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1040,30 +1205,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1077,13 +1242,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1097,13 +1262,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1117,13 +1282,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1137,13 +1302,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1157,13 +1322,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -1177,13 +1342,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -1197,13 +1362,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1217,13 +1382,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -1237,13 +1402,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -1257,13 +1422,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1277,13 +1442,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1297,13 +1462,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1317,13 +1482,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -1337,13 +1502,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1357,13 +1522,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1377,13 +1542,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -1397,13 +1562,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="D19">
         <v>5</v>
@@ -1417,13 +1582,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1437,13 +1602,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -1455,7 +1620,1607 @@
         <v>12000</v>
       </c>
     </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>3826</v>
+      </c>
+      <c r="F22">
+        <v>11478</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>25786</v>
+      </c>
+      <c r="F23">
+        <v>77358</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>45776</v>
+      </c>
+      <c r="F24">
+        <v>137328</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>24069</v>
+      </c>
+      <c r="F25">
+        <v>48138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>37197</v>
+      </c>
+      <c r="F26">
+        <v>37197</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>42731</v>
+      </c>
+      <c r="F27">
+        <v>42731</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>9669</v>
+      </c>
+      <c r="F28">
+        <v>9669</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>33420</v>
+      </c>
+      <c r="F29">
+        <v>33420</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>44651</v>
+      </c>
+      <c r="F30">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>33713</v>
+      </c>
+      <c r="F31">
+        <v>101139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>7879</v>
+      </c>
+      <c r="F32">
+        <v>15758</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>8822</v>
+      </c>
+      <c r="F33">
+        <v>26466</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>17857</v>
+      </c>
+      <c r="F34">
+        <v>35714</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>36823</v>
+      </c>
+      <c r="F35">
+        <v>110469</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>2175</v>
+      </c>
+      <c r="F36">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>10159</v>
+      </c>
+      <c r="F37">
+        <v>20318</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <v>7121</v>
+      </c>
+      <c r="F38">
+        <v>21363</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>41951</v>
+      </c>
+      <c r="F39">
+        <v>125853</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>2332</v>
+      </c>
+      <c r="F40">
+        <v>2332</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>33556</v>
+      </c>
+      <c r="F41">
+        <v>33556</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>25534</v>
+      </c>
+      <c r="F42">
+        <v>51068</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>6565</v>
+      </c>
+      <c r="F43">
+        <v>6565</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>20447</v>
+      </c>
+      <c r="F44">
+        <v>20447</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <v>33796</v>
+      </c>
+      <c r="F45">
+        <v>101388</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>38601</v>
+      </c>
+      <c r="F46">
+        <v>77202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>47110</v>
+      </c>
+      <c r="F47">
+        <v>141330</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>28175</v>
+      </c>
+      <c r="F48">
+        <v>28175</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>17870</v>
+      </c>
+      <c r="F49">
+        <v>35740</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>27065</v>
+      </c>
+      <c r="F50">
+        <v>27065</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" t="s">
+        <v>31</v>
+      </c>
+      <c r="C51" t="s">
+        <v>78</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>14646</v>
+      </c>
+      <c r="F51">
+        <v>14646</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D52">
+        <v>3</v>
+      </c>
+      <c r="E52">
+        <v>43775</v>
+      </c>
+      <c r="F52">
+        <v>131325</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" t="s">
+        <v>80</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>4902</v>
+      </c>
+      <c r="F53">
+        <v>4902</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>41186</v>
+      </c>
+      <c r="F54">
+        <v>82372</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>40948</v>
+      </c>
+      <c r="F55">
+        <v>81896</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="E56">
+        <v>32403</v>
+      </c>
+      <c r="F56">
+        <v>97209</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+      <c r="E57">
+        <v>21628</v>
+      </c>
+      <c r="F57">
+        <v>64884</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" t="s">
+        <v>74</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>10989</v>
+      </c>
+      <c r="F58">
+        <v>10989</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" t="s">
+        <v>78</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>16693</v>
+      </c>
+      <c r="F59">
+        <v>16693</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" t="s">
+        <v>85</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>16748</v>
+      </c>
+      <c r="F60">
+        <v>33496</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" t="s">
+        <v>86</v>
+      </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+      <c r="E61">
+        <v>8802</v>
+      </c>
+      <c r="F61">
+        <v>26406</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="E62">
+        <v>25629</v>
+      </c>
+      <c r="F62">
+        <v>76887</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" t="s">
+        <v>88</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>22106</v>
+      </c>
+      <c r="F63">
+        <v>44212</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64" t="s">
+        <v>55</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>12023</v>
+      </c>
+      <c r="F64">
+        <v>12023</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B65" t="s">
+        <v>39</v>
+      </c>
+      <c r="C65" t="s">
+        <v>85</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <v>28626</v>
+      </c>
+      <c r="F65">
+        <v>57252</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66" t="s">
+        <v>36</v>
+      </c>
+      <c r="C66" t="s">
+        <v>89</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66">
+        <v>16072</v>
+      </c>
+      <c r="F66">
+        <v>32144</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" t="s">
+        <v>40</v>
+      </c>
+      <c r="C67" t="s">
+        <v>90</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>11663</v>
+      </c>
+      <c r="F67">
+        <v>23326</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68" t="s">
+        <v>40</v>
+      </c>
+      <c r="C68" t="s">
+        <v>58</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="E68">
+        <v>44321</v>
+      </c>
+      <c r="F68">
+        <v>132963</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69" t="s">
+        <v>32</v>
+      </c>
+      <c r="C69" t="s">
+        <v>91</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>41920</v>
+      </c>
+      <c r="F69">
+        <v>41920</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" t="s">
+        <v>92</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <v>8877</v>
+      </c>
+      <c r="F70">
+        <v>17754</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" t="s">
+        <v>32</v>
+      </c>
+      <c r="C71" t="s">
+        <v>93</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>36712</v>
+      </c>
+      <c r="F71">
+        <v>36712</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72" t="s">
+        <v>86</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <v>16113</v>
+      </c>
+      <c r="F72">
+        <v>32226</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>18</v>
+      </c>
+      <c r="B73" t="s">
+        <v>31</v>
+      </c>
+      <c r="C73" t="s">
+        <v>94</v>
+      </c>
+      <c r="D73">
+        <v>3</v>
+      </c>
+      <c r="E73">
+        <v>11444</v>
+      </c>
+      <c r="F73">
+        <v>34332</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" t="s">
+        <v>36</v>
+      </c>
+      <c r="C74" t="s">
+        <v>95</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+      <c r="E74">
+        <v>13823</v>
+      </c>
+      <c r="F74">
+        <v>27646</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75" t="s">
+        <v>40</v>
+      </c>
+      <c r="C75" t="s">
+        <v>96</v>
+      </c>
+      <c r="D75">
+        <v>3</v>
+      </c>
+      <c r="E75">
+        <v>3213</v>
+      </c>
+      <c r="F75">
+        <v>9639</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" t="s">
+        <v>36</v>
+      </c>
+      <c r="C76" t="s">
+        <v>91</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>35704</v>
+      </c>
+      <c r="F76">
+        <v>71408</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" t="s">
+        <v>37</v>
+      </c>
+      <c r="C77" t="s">
+        <v>84</v>
+      </c>
+      <c r="D77">
+        <v>3</v>
+      </c>
+      <c r="E77">
+        <v>32597</v>
+      </c>
+      <c r="F77">
+        <v>97791</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>20</v>
+      </c>
+      <c r="B78" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" t="s">
+        <v>60</v>
+      </c>
+      <c r="D78">
+        <v>3</v>
+      </c>
+      <c r="E78">
+        <v>42842</v>
+      </c>
+      <c r="F78">
+        <v>128526</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79" t="s">
+        <v>32</v>
+      </c>
+      <c r="C79" t="s">
+        <v>97</v>
+      </c>
+      <c r="D79">
+        <v>3</v>
+      </c>
+      <c r="E79">
+        <v>12865</v>
+      </c>
+      <c r="F79">
+        <v>38595</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>20</v>
+      </c>
+      <c r="B80" t="s">
+        <v>40</v>
+      </c>
+      <c r="C80" t="s">
+        <v>96</v>
+      </c>
+      <c r="D80">
+        <v>2</v>
+      </c>
+      <c r="E80">
+        <v>8833</v>
+      </c>
+      <c r="F80">
+        <v>17666</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>20</v>
+      </c>
+      <c r="B81" t="s">
+        <v>32</v>
+      </c>
+      <c r="C81" t="s">
+        <v>98</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>45142</v>
+      </c>
+      <c r="F81">
+        <v>45142</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>21</v>
+      </c>
+      <c r="B82" t="s">
+        <v>39</v>
+      </c>
+      <c r="C82" t="s">
+        <v>99</v>
+      </c>
+      <c r="D82">
+        <v>2</v>
+      </c>
+      <c r="E82">
+        <v>38864</v>
+      </c>
+      <c r="F82">
+        <v>77728</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>21</v>
+      </c>
+      <c r="B83" t="s">
+        <v>36</v>
+      </c>
+      <c r="C83" t="s">
+        <v>100</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>24832</v>
+      </c>
+      <c r="F83">
+        <v>24832</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>21</v>
+      </c>
+      <c r="B84" t="s">
+        <v>37</v>
+      </c>
+      <c r="C84" t="s">
+        <v>93</v>
+      </c>
+      <c r="D84">
+        <v>3</v>
+      </c>
+      <c r="E84">
+        <v>15459</v>
+      </c>
+      <c r="F84">
+        <v>46377</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" t="s">
+        <v>34</v>
+      </c>
+      <c r="C85" t="s">
+        <v>96</v>
+      </c>
+      <c r="D85">
+        <v>3</v>
+      </c>
+      <c r="E85">
+        <v>41059</v>
+      </c>
+      <c r="F85">
+        <v>123177</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>22</v>
+      </c>
+      <c r="B86" t="s">
+        <v>38</v>
+      </c>
+      <c r="C86" t="s">
+        <v>101</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>28097</v>
+      </c>
+      <c r="F86">
+        <v>28097</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>22</v>
+      </c>
+      <c r="B87" t="s">
+        <v>32</v>
+      </c>
+      <c r="C87" t="s">
+        <v>102</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>20212</v>
+      </c>
+      <c r="F87">
+        <v>20212</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>22</v>
+      </c>
+      <c r="B88" t="s">
+        <v>38</v>
+      </c>
+      <c r="C88" t="s">
+        <v>103</v>
+      </c>
+      <c r="D88">
+        <v>2</v>
+      </c>
+      <c r="E88">
+        <v>12833</v>
+      </c>
+      <c r="F88">
+        <v>25666</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>22</v>
+      </c>
+      <c r="B89" t="s">
+        <v>34</v>
+      </c>
+      <c r="C89" t="s">
+        <v>104</v>
+      </c>
+      <c r="D89">
+        <v>3</v>
+      </c>
+      <c r="E89">
+        <v>24929</v>
+      </c>
+      <c r="F89">
+        <v>74787</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>23</v>
+      </c>
+      <c r="B90" t="s">
+        <v>36</v>
+      </c>
+      <c r="C90" t="s">
+        <v>105</v>
+      </c>
+      <c r="D90">
+        <v>3</v>
+      </c>
+      <c r="E90">
+        <v>45797</v>
+      </c>
+      <c r="F90">
+        <v>137391</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>23</v>
+      </c>
+      <c r="B91" t="s">
+        <v>37</v>
+      </c>
+      <c r="C91" t="s">
+        <v>106</v>
+      </c>
+      <c r="D91">
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <v>34560</v>
+      </c>
+      <c r="F91">
+        <v>69120</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>23</v>
+      </c>
+      <c r="B92" t="s">
+        <v>40</v>
+      </c>
+      <c r="C92" t="s">
+        <v>104</v>
+      </c>
+      <c r="D92">
+        <v>2</v>
+      </c>
+      <c r="E92">
+        <v>32218</v>
+      </c>
+      <c r="F92">
+        <v>64436</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" t="s">
+        <v>36</v>
+      </c>
+      <c r="C93" t="s">
+        <v>107</v>
+      </c>
+      <c r="D93">
+        <v>2</v>
+      </c>
+      <c r="E93">
+        <v>28430</v>
+      </c>
+      <c r="F93">
+        <v>56860</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94" t="s">
+        <v>39</v>
+      </c>
+      <c r="C94" t="s">
+        <v>108</v>
+      </c>
+      <c r="D94">
+        <v>3</v>
+      </c>
+      <c r="E94">
+        <v>41819</v>
+      </c>
+      <c r="F94">
+        <v>125457</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>24</v>
+      </c>
+      <c r="B95" t="s">
+        <v>31</v>
+      </c>
+      <c r="C95" t="s">
+        <v>109</v>
+      </c>
+      <c r="D95">
+        <v>3</v>
+      </c>
+      <c r="E95">
+        <v>7460</v>
+      </c>
+      <c r="F95">
+        <v>22380</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>24</v>
+      </c>
+      <c r="B96" t="s">
+        <v>38</v>
+      </c>
+      <c r="C96" t="s">
+        <v>100</v>
+      </c>
+      <c r="D96">
+        <v>3</v>
+      </c>
+      <c r="E96">
+        <v>11391</v>
+      </c>
+      <c r="F96">
+        <v>34173</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>24</v>
+      </c>
+      <c r="B97" t="s">
+        <v>39</v>
+      </c>
+      <c r="C97" t="s">
+        <v>110</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>21686</v>
+      </c>
+      <c r="F97">
+        <v>21686</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>25</v>
+      </c>
+      <c r="B98" t="s">
+        <v>34</v>
+      </c>
+      <c r="C98" t="s">
+        <v>111</v>
+      </c>
+      <c r="D98">
+        <v>3</v>
+      </c>
+      <c r="E98">
+        <v>41589</v>
+      </c>
+      <c r="F98">
+        <v>124767</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>25</v>
+      </c>
+      <c r="B99" t="s">
+        <v>38</v>
+      </c>
+      <c r="C99" t="s">
+        <v>102</v>
+      </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
+      <c r="E99">
+        <v>10623</v>
+      </c>
+      <c r="F99">
+        <v>21246</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>25</v>
+      </c>
+      <c r="B100" t="s">
+        <v>40</v>
+      </c>
+      <c r="C100" t="s">
+        <v>112</v>
+      </c>
+      <c r="D100">
+        <v>3</v>
+      </c>
+      <c r="E100">
+        <v>17256</v>
+      </c>
+      <c r="F100">
+        <v>51768</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>25</v>
+      </c>
+      <c r="B101" t="s">
+        <v>37</v>
+      </c>
+      <c r="C101" t="s">
+        <v>113</v>
+      </c>
+      <c r="D101">
+        <v>3</v>
+      </c>
+      <c r="E101">
+        <v>9979</v>
+      </c>
+      <c r="F101">
+        <v>29937</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>